<commit_message>
Versão 5 do índice Nupe das empresas cearenses listadas em bolsa.
1 - Inclusão do script versão 3.

A ser incluido:

1 - Arquivo com os dados para divulgação;
2 - Criação de painel no Power BI
</commit_message>
<xml_diff>
--- a/data/empresas_na_bolsa_FCA.xlsx
+++ b/data/empresas_na_bolsa_FCA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{5F3F4C7E-942E-4478-A31A-3B8DD3609DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2B151F3-150A-4990-8A9B-0221F88B4491}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:40009_{5F3F4C7E-942E-4478-A31A-3B8DD3609DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02A1F388-849A-40CF-ADC0-BC85DB67C95E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7633,7 +7633,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8160,7 +8160,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{23A3FDF7-EE8B-4445-ABB0-6855DC305844}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8473,7 +8475,7 @@
   <dimension ref="A1:S429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C405" sqref="C405"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>